<commit_message>
[Fix] Proceedings filters and download file
</commit_message>
<xml_diff>
--- a/Service.MedicalRecord/wwwroot/layout/excel/expediente/ExpedienteListado.xlsx
+++ b/Service.MedicalRecord/wwwroot/layout/excel/expediente/ExpedienteListado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ResposAxsis\API\Service.MedicalRecord\wwwroot\layout\excel\expediente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\workspace\axsis\LabRamos\API\Service.MedicalRecord\wwwroot\layout\excel\expediente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD7C26C-0A8B-48BE-AEE5-BE5A81B4D686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6066DE3-660D-4506-8B32-4760A57959CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="465" windowWidth="18000" windowHeight="9270" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Expedientes" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,45 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nombre</t>
+  </si>
+  <si>
+    <t>Expediente</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>{{item.Expediente}}</t>
+  </si>
+  <si>
+    <t>{{item.NomprePaciente}}</t>
+  </si>
+  <si>
+    <t>{{item.Edad}}</t>
+  </si>
+  <si>
+    <t>{{item.Telefono}}</t>
+  </si>
+  <si>
+    <t>{{item.FechaNacimiento}}</t>
+  </si>
+  <si>
+    <t>{{item.MonederoElectronico}}</t>
+  </si>
+  <si>
+    <t>{{item.Genero}}</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>Monedero electrónico</t>
   </si>
   <si>
     <r>
@@ -68,47 +107,8 @@
         <scheme val="minor"/>
       </rPr>
       <t>Listado de {{Titulo}}
-DEL {{Fecha}} AL {{Fecha}}</t>
+DEL {{FechaInicial}} AL {{FechaFinal}}</t>
     </r>
-  </si>
-  <si>
-    <t>Expediente</t>
-  </si>
-  <si>
-    <t>Genero</t>
-  </si>
-  <si>
-    <t>Edad</t>
-  </si>
-  <si>
-    <t>Fecha de nacimiento</t>
-  </si>
-  <si>
-    <t>{{item.Expediente}}</t>
-  </si>
-  <si>
-    <t>{{item.NomprePaciente}}</t>
-  </si>
-  <si>
-    <t>{{item.Edad}}</t>
-  </si>
-  <si>
-    <t>{{item.Telefono}}</t>
-  </si>
-  <si>
-    <t>{{item.FechaNacimiento}}</t>
-  </si>
-  <si>
-    <t>{{item.MonederoElectronico}}</t>
-  </si>
-  <si>
-    <t>{{item.Genero}}</t>
-  </si>
-  <si>
-    <t>Teléfono</t>
-  </si>
-  <si>
-    <t>Monedero electrónico</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -591,48 +591,48 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>